<commit_message>
Final commit before sharing with WFU
</commit_message>
<xml_diff>
--- a/Dendro_data_supporting/Dendro_metadata.xlsx
+++ b/Dendro_data_supporting/Dendro_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://luky-my.sharepoint.com/personal/drva228_uky_edu/Documents/TMCF/Continuous_data/TMCF_Dendrometers/Dendro_data_supporting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="211" documentId="13_ncr:1_{98E03C99-2F99-44D8-9D25-7388A4E8D3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3D733C5-B437-4A2C-8BD3-4EF64D187A66}"/>
+  <xr:revisionPtr revIDLastSave="216" documentId="13_ncr:1_{98E03C99-2F99-44D8-9D25-7388A4E8D3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51D17A2C-A5DF-45A7-A329-8404AF5EF1DE}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{937AFFAC-D172-4152-98E4-CB2C6927A2FA}"/>
   </bookViews>
@@ -38,12 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="82">
   <si>
-    <t>TreeID</t>
-  </si>
-  <si>
-    <t>Dendro.Num</t>
-  </si>
-  <si>
     <t>ET1</t>
   </si>
   <si>
@@ -146,9 +140,6 @@
     <t>2022-07-28 18:15:00</t>
   </si>
   <si>
-    <t>DendroID</t>
-  </si>
-  <si>
     <t>2022-08-22 14:00:00</t>
   </si>
   <si>
@@ -282,6 +273,15 @@
   </si>
   <si>
     <t>77</t>
+  </si>
+  <si>
+    <t>Tree</t>
+  </si>
+  <si>
+    <t>Dendrometer</t>
+  </si>
+  <si>
+    <t>Letter</t>
   </si>
 </sst>
 </file>
@@ -323,11 +323,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -645,665 +643,666 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="18.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>81</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>80</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C2" t="str">
         <f>_xlfn.CONCAT(A2, B2)</f>
         <v>ET1a</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C29" si="0">_xlfn.CONCAT(A3, B3)</f>
         <v>ET2a</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>ET2b</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C4" t="str">
-        <f t="shared" si="0"/>
-        <v>ET2b</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>ET3a</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" t="s">
         <v>44</v>
-      </c>
-      <c r="C5" t="str">
-        <f t="shared" si="0"/>
-        <v>ET3a</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G5" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
         <v>ET4a</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
         <v>ET4b</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>ET5a</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" t="s">
         <v>44</v>
       </c>
-      <c r="C8" t="str">
-        <f t="shared" si="0"/>
-        <v>ET5a</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="2" t="str">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" t="str">
         <f t="shared" si="0"/>
         <v>ET5b</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="2" t="s">
+      <c r="D9" s="1" t="s">
         <v>49</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G9" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>ET6a</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" t="s">
         <v>44</v>
-      </c>
-      <c r="C10" t="str">
-        <f t="shared" si="0"/>
-        <v>ET6a</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G10" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>ET7a</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" t="s">
         <v>44</v>
-      </c>
-      <c r="C11" t="str">
-        <f t="shared" si="0"/>
-        <v>ET7a</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G11" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>ET8a</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" t="s">
         <v>44</v>
-      </c>
-      <c r="C12" t="str">
-        <f t="shared" si="0"/>
-        <v>ET8a</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G12" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>FB1a</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G13" t="s">
         <v>44</v>
-      </c>
-      <c r="C13" t="str">
-        <f t="shared" si="0"/>
-        <v>FB1a</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G13" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>FB2a</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" t="s">
         <v>44</v>
-      </c>
-      <c r="C14" t="str">
-        <f t="shared" si="0"/>
-        <v>FB2a</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G14" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
         <v>FB3a</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G15" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
         <v>FB3b</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G16" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
         <v>FB4a</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G17" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
         <v>FB4b</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G18" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
         <v>FB5a</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G19" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
         <v>FB5b</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G20" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
         <v>FB6a</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G21" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
         <v>FB6b</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G22" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>FB7a</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G23" t="s">
         <v>44</v>
-      </c>
-      <c r="C23" t="str">
-        <f t="shared" si="0"/>
-        <v>FB7a</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G23" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
         <v>FB7b</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G24" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>FB8a</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G25" t="s">
         <v>44</v>
-      </c>
-      <c r="C25" t="str">
-        <f t="shared" si="0"/>
-        <v>FB8a</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G25" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>TV1a</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G26" t="s">
         <v>44</v>
-      </c>
-      <c r="C26" t="str">
-        <f t="shared" si="0"/>
-        <v>TV1a</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G26" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B27" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>TV2a</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G27" t="s">
         <v>44</v>
-      </c>
-      <c r="C27" t="str">
-        <f t="shared" si="0"/>
-        <v>TV2a</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G27" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>TV3a</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G28" t="s">
         <v>44</v>
-      </c>
-      <c r="C28" t="str">
-        <f t="shared" si="0"/>
-        <v>TV3a</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G28" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>TV4a</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G29" t="s">
         <v>44</v>
-      </c>
-      <c r="C29" t="str">
-        <f t="shared" si="0"/>
-        <v>TV4a</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G29" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>